<commit_message>
Nya protokoll och editering av horseorde(ej klart)
</commit_message>
<xml_diff>
--- a/mallar/Protokoll/Protokoll_2019_Pas_de_deux_klass(mall).xlsx
+++ b/mallar/Protokoll/Protokoll_2019_Pas_de_deux_klass(mall).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magnus.sandberg\Documents\Visual Studio 2015\Projects\VoltigeClosedXML\mallar\Protokoll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E91357-4A37-473D-8521-04107DD41CB0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC61B24C-5031-4E2F-BB61-96F424528E73}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1837" yWindow="1837" windowWidth="16201" windowHeight="9398" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="24" r:id="rId1"/>
@@ -1639,7 +1639,7 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="279">
+  <cellXfs count="280">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2048,14 +2048,170 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="9"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="4" borderId="37" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="4" borderId="28" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="4" borderId="47" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="10" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="37" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="27" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2064,174 +2220,100 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="169" fontId="2" fillId="0" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="4" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="4" borderId="37" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="4" borderId="28" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="4" borderId="47" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="10" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="37" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="27" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2241,94 +2323,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="3" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="4" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2368,6 +2368,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Dezimal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2751,8 +2752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -3433,8 +3434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" view="pageLayout" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -3499,10 +3500,10 @@
         <v>13</v>
       </c>
       <c r="B5" s="156"/>
-      <c r="C5" s="216"/>
-      <c r="D5" s="216"/>
-      <c r="E5" s="216"/>
-      <c r="F5" s="216"/>
+      <c r="C5" s="170"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="170"/>
+      <c r="F5" s="170"/>
       <c r="H5" s="160"/>
       <c r="I5" s="159" t="s">
         <v>11</v>
@@ -3524,68 +3525,68 @@
         <v>146</v>
       </c>
       <c r="B7" s="156"/>
-      <c r="C7" s="216"/>
-      <c r="D7" s="216"/>
-      <c r="E7" s="216"/>
-      <c r="F7" s="216"/>
+      <c r="C7" s="170"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="170"/>
+      <c r="F7" s="170"/>
       <c r="H7" s="136" t="s">
         <v>145</v>
       </c>
-      <c r="I7" s="228"/>
-      <c r="J7" s="229"/>
-      <c r="K7" s="229"/>
-      <c r="L7" s="229"/>
+      <c r="I7" s="173"/>
+      <c r="J7" s="174"/>
+      <c r="K7" s="174"/>
+      <c r="L7" s="174"/>
     </row>
     <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="136" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="136"/>
-      <c r="C8" s="230"/>
-      <c r="D8" s="230"/>
-      <c r="E8" s="230"/>
-      <c r="F8" s="230"/>
+      <c r="C8" s="175"/>
+      <c r="D8" s="175"/>
+      <c r="E8" s="175"/>
+      <c r="F8" s="175"/>
       <c r="H8" s="156" t="s">
         <v>144</v>
       </c>
-      <c r="I8" s="231"/>
-      <c r="J8" s="232"/>
-      <c r="K8" s="232"/>
-      <c r="L8" s="232"/>
+      <c r="I8" s="176"/>
+      <c r="J8" s="177"/>
+      <c r="K8" s="177"/>
+      <c r="L8" s="177"/>
     </row>
     <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="156" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="156"/>
-      <c r="C9" s="216"/>
-      <c r="D9" s="216"/>
-      <c r="E9" s="216"/>
-      <c r="F9" s="216"/>
-      <c r="I9" s="217"/>
-      <c r="J9" s="218"/>
-      <c r="K9" s="218"/>
-      <c r="L9" s="218"/>
+      <c r="C9" s="170"/>
+      <c r="D9" s="170"/>
+      <c r="E9" s="170"/>
+      <c r="F9" s="170"/>
+      <c r="I9" s="171"/>
+      <c r="J9" s="172"/>
+      <c r="K9" s="172"/>
+      <c r="L9" s="172"/>
     </row>
     <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="156" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="156"/>
-      <c r="C10" s="216"/>
-      <c r="D10" s="216"/>
-      <c r="E10" s="216"/>
-      <c r="F10" s="216"/>
-      <c r="I10" s="217"/>
-      <c r="J10" s="218"/>
-      <c r="K10" s="218"/>
-      <c r="L10" s="218"/>
+      <c r="C10" s="170"/>
+      <c r="D10" s="170"/>
+      <c r="E10" s="170"/>
+      <c r="F10" s="170"/>
+      <c r="I10" s="171"/>
+      <c r="J10" s="172"/>
+      <c r="K10" s="172"/>
+      <c r="L10" s="172"/>
     </row>
     <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I11" s="217"/>
-      <c r="J11" s="218"/>
-      <c r="K11" s="218"/>
-      <c r="L11" s="218"/>
+      <c r="I11" s="171"/>
+      <c r="J11" s="172"/>
+      <c r="K11" s="172"/>
+      <c r="L11" s="172"/>
     </row>
     <row r="12" spans="1:13" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A12" s="155" t="s">
@@ -3597,95 +3598,95 @@
       <c r="E12" s="35"/>
       <c r="F12" s="35"/>
       <c r="G12" s="35"/>
-      <c r="H12" s="219" t="s">
+      <c r="H12" s="187" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="220"/>
-      <c r="J12" s="221" t="s">
+      <c r="I12" s="188"/>
+      <c r="J12" s="189" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="222"/>
-      <c r="L12" s="223"/>
+      <c r="K12" s="190"/>
+      <c r="L12" s="191"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="188" t="s">
+      <c r="A13" s="178" t="s">
         <v>143</v>
       </c>
-      <c r="B13" s="207" t="s">
+      <c r="B13" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="207" t="s">
+      <c r="C13" s="181" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="207"/>
-      <c r="E13" s="207"/>
-      <c r="F13" s="193" t="s">
+      <c r="D13" s="181"/>
+      <c r="E13" s="181"/>
+      <c r="F13" s="183" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="225"/>
-      <c r="H13" s="226"/>
-      <c r="I13" s="227"/>
-      <c r="J13" s="213">
+      <c r="G13" s="184"/>
+      <c r="H13" s="185"/>
+      <c r="I13" s="186"/>
+      <c r="J13" s="203">
         <v>0.2</v>
       </c>
-      <c r="K13" s="202"/>
-      <c r="L13" s="205">
+      <c r="K13" s="192"/>
+      <c r="L13" s="195">
         <f>K13*0.2</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="224"/>
-      <c r="B14" s="207"/>
-      <c r="C14" s="207" t="s">
+      <c r="A14" s="179"/>
+      <c r="B14" s="181"/>
+      <c r="C14" s="181" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="207"/>
-      <c r="E14" s="207"/>
-      <c r="F14" s="208" t="s">
+      <c r="D14" s="181"/>
+      <c r="E14" s="181"/>
+      <c r="F14" s="197" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="209"/>
-      <c r="H14" s="195"/>
-      <c r="I14" s="196"/>
-      <c r="J14" s="214"/>
-      <c r="K14" s="203"/>
-      <c r="L14" s="205"/>
+      <c r="G14" s="198"/>
+      <c r="H14" s="199"/>
+      <c r="I14" s="200"/>
+      <c r="J14" s="204"/>
+      <c r="K14" s="193"/>
+      <c r="L14" s="195"/>
     </row>
     <row r="15" spans="1:13" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="189"/>
-      <c r="B15" s="210"/>
-      <c r="C15" s="210" t="s">
+      <c r="A15" s="180"/>
+      <c r="B15" s="182"/>
+      <c r="C15" s="182" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="210"/>
-      <c r="E15" s="210"/>
-      <c r="F15" s="208" t="s">
+      <c r="D15" s="182"/>
+      <c r="E15" s="182"/>
+      <c r="F15" s="197" t="s">
         <v>142</v>
       </c>
-      <c r="G15" s="209"/>
-      <c r="H15" s="211"/>
-      <c r="I15" s="212"/>
-      <c r="J15" s="215"/>
-      <c r="K15" s="204"/>
-      <c r="L15" s="206"/>
+      <c r="G15" s="198"/>
+      <c r="H15" s="201"/>
+      <c r="I15" s="202"/>
+      <c r="J15" s="205"/>
+      <c r="K15" s="194"/>
+      <c r="L15" s="196"/>
     </row>
     <row r="16" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="188" t="s">
+      <c r="A16" s="178" t="s">
         <v>141</v>
       </c>
-      <c r="B16" s="190" t="s">
+      <c r="B16" s="206" t="s">
         <v>140</v>
       </c>
-      <c r="C16" s="191"/>
-      <c r="D16" s="191"/>
-      <c r="E16" s="192"/>
-      <c r="F16" s="193" t="s">
+      <c r="C16" s="207"/>
+      <c r="D16" s="207"/>
+      <c r="E16" s="208"/>
+      <c r="F16" s="183" t="s">
         <v>139</v>
       </c>
-      <c r="G16" s="194"/>
-      <c r="H16" s="195"/>
-      <c r="I16" s="196"/>
+      <c r="G16" s="209"/>
+      <c r="H16" s="199"/>
+      <c r="I16" s="200"/>
       <c r="J16" s="154">
         <v>0.4</v>
       </c>
@@ -3697,19 +3698,19 @@
       <c r="M16" s="130"/>
     </row>
     <row r="17" spans="1:12" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="189"/>
-      <c r="B17" s="197" t="s">
+      <c r="A17" s="180"/>
+      <c r="B17" s="210" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="198"/>
-      <c r="D17" s="198"/>
-      <c r="E17" s="199"/>
-      <c r="F17" s="200" t="s">
+      <c r="C17" s="211"/>
+      <c r="D17" s="211"/>
+      <c r="E17" s="212"/>
+      <c r="F17" s="213" t="s">
         <v>44</v>
       </c>
-      <c r="G17" s="201"/>
-      <c r="H17" s="195"/>
-      <c r="I17" s="196"/>
+      <c r="G17" s="214"/>
+      <c r="H17" s="199"/>
+      <c r="I17" s="200"/>
       <c r="J17" s="154">
         <v>0.4</v>
       </c>
@@ -3723,17 +3724,17 @@
       <c r="A18" s="151" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="176" t="s">
+      <c r="B18" s="215" t="s">
         <v>138</v>
       </c>
-      <c r="C18" s="177"/>
-      <c r="D18" s="177"/>
-      <c r="E18" s="177"/>
-      <c r="F18" s="177"/>
-      <c r="G18" s="177"/>
-      <c r="H18" s="177"/>
-      <c r="I18" s="177"/>
-      <c r="J18" s="178"/>
+      <c r="C18" s="216"/>
+      <c r="D18" s="216"/>
+      <c r="E18" s="216"/>
+      <c r="F18" s="216"/>
+      <c r="G18" s="216"/>
+      <c r="H18" s="216"/>
+      <c r="I18" s="216"/>
+      <c r="J18" s="217"/>
       <c r="K18" s="150"/>
       <c r="L18" s="149"/>
     </row>
@@ -3751,90 +3752,90 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="179" t="s">
+      <c r="A21" s="218" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="180"/>
-      <c r="C21" s="180"/>
-      <c r="D21" s="180"/>
-      <c r="E21" s="180"/>
-      <c r="F21" s="180"/>
-      <c r="G21" s="180"/>
-      <c r="H21" s="180"/>
-      <c r="I21" s="180"/>
-      <c r="J21" s="180"/>
-      <c r="K21" s="180"/>
-      <c r="L21" s="181"/>
+      <c r="B21" s="219"/>
+      <c r="C21" s="219"/>
+      <c r="D21" s="219"/>
+      <c r="E21" s="219"/>
+      <c r="F21" s="219"/>
+      <c r="G21" s="219"/>
+      <c r="H21" s="219"/>
+      <c r="I21" s="219"/>
+      <c r="J21" s="219"/>
+      <c r="K21" s="219"/>
+      <c r="L21" s="220"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="182"/>
-      <c r="B22" s="183"/>
-      <c r="C22" s="183"/>
-      <c r="D22" s="183"/>
-      <c r="E22" s="183"/>
-      <c r="F22" s="183"/>
-      <c r="G22" s="183"/>
-      <c r="H22" s="183"/>
-      <c r="I22" s="183"/>
-      <c r="J22" s="183"/>
-      <c r="K22" s="183"/>
-      <c r="L22" s="184"/>
+      <c r="A22" s="221"/>
+      <c r="B22" s="222"/>
+      <c r="C22" s="222"/>
+      <c r="D22" s="222"/>
+      <c r="E22" s="222"/>
+      <c r="F22" s="222"/>
+      <c r="G22" s="222"/>
+      <c r="H22" s="222"/>
+      <c r="I22" s="222"/>
+      <c r="J22" s="222"/>
+      <c r="K22" s="222"/>
+      <c r="L22" s="223"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="182"/>
-      <c r="B23" s="183"/>
-      <c r="C23" s="183"/>
-      <c r="D23" s="183"/>
-      <c r="E23" s="183"/>
-      <c r="F23" s="183"/>
-      <c r="G23" s="183"/>
-      <c r="H23" s="183"/>
-      <c r="I23" s="183"/>
-      <c r="J23" s="183"/>
-      <c r="K23" s="183"/>
-      <c r="L23" s="184"/>
+      <c r="A23" s="221"/>
+      <c r="B23" s="222"/>
+      <c r="C23" s="222"/>
+      <c r="D23" s="222"/>
+      <c r="E23" s="222"/>
+      <c r="F23" s="222"/>
+      <c r="G23" s="222"/>
+      <c r="H23" s="222"/>
+      <c r="I23" s="222"/>
+      <c r="J23" s="222"/>
+      <c r="K23" s="222"/>
+      <c r="L23" s="223"/>
     </row>
     <row r="24" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="182"/>
-      <c r="B24" s="183"/>
-      <c r="C24" s="183"/>
-      <c r="D24" s="183"/>
-      <c r="E24" s="183"/>
-      <c r="F24" s="183"/>
-      <c r="G24" s="183"/>
-      <c r="H24" s="183"/>
-      <c r="I24" s="183"/>
-      <c r="J24" s="183"/>
-      <c r="K24" s="183"/>
-      <c r="L24" s="184"/>
+      <c r="A24" s="221"/>
+      <c r="B24" s="222"/>
+      <c r="C24" s="222"/>
+      <c r="D24" s="222"/>
+      <c r="E24" s="222"/>
+      <c r="F24" s="222"/>
+      <c r="G24" s="222"/>
+      <c r="H24" s="222"/>
+      <c r="I24" s="222"/>
+      <c r="J24" s="222"/>
+      <c r="K24" s="222"/>
+      <c r="L24" s="223"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="185"/>
-      <c r="B25" s="186"/>
-      <c r="C25" s="186"/>
-      <c r="D25" s="186"/>
-      <c r="E25" s="186"/>
-      <c r="F25" s="186"/>
-      <c r="G25" s="186"/>
-      <c r="H25" s="186"/>
-      <c r="I25" s="186"/>
-      <c r="J25" s="186"/>
-      <c r="K25" s="186"/>
-      <c r="L25" s="187"/>
+      <c r="A25" s="224"/>
+      <c r="B25" s="225"/>
+      <c r="C25" s="225"/>
+      <c r="D25" s="225"/>
+      <c r="E25" s="225"/>
+      <c r="F25" s="225"/>
+      <c r="G25" s="225"/>
+      <c r="H25" s="225"/>
+      <c r="I25" s="225"/>
+      <c r="J25" s="225"/>
+      <c r="K25" s="225"/>
+      <c r="L25" s="226"/>
     </row>
     <row r="27" spans="1:12" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="173" t="s">
+      <c r="A27" s="227" t="s">
         <v>136</v>
       </c>
-      <c r="B27" s="173"/>
-      <c r="C27" s="173"/>
-      <c r="D27" s="173"/>
-      <c r="E27" s="173"/>
-      <c r="F27" s="173"/>
-      <c r="G27" s="173"/>
-      <c r="H27" s="173"/>
-      <c r="I27" s="174"/>
-      <c r="J27" s="174"/>
+      <c r="B27" s="227"/>
+      <c r="C27" s="227"/>
+      <c r="D27" s="227"/>
+      <c r="E27" s="227"/>
+      <c r="F27" s="227"/>
+      <c r="G27" s="227"/>
+      <c r="H27" s="227"/>
+      <c r="I27" s="228"/>
+      <c r="J27" s="228"/>
       <c r="K27" s="146" t="s">
         <v>134</v>
       </c>
@@ -3844,18 +3845,18 @@
       </c>
     </row>
     <row r="28" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="173" t="s">
+      <c r="A28" s="227" t="s">
         <v>135</v>
       </c>
-      <c r="B28" s="173"/>
-      <c r="C28" s="173"/>
-      <c r="D28" s="173"/>
-      <c r="E28" s="173"/>
-      <c r="F28" s="173"/>
-      <c r="G28" s="173"/>
-      <c r="H28" s="173"/>
-      <c r="I28" s="174"/>
-      <c r="J28" s="174"/>
+      <c r="B28" s="227"/>
+      <c r="C28" s="227"/>
+      <c r="D28" s="227"/>
+      <c r="E28" s="227"/>
+      <c r="F28" s="227"/>
+      <c r="G28" s="227"/>
+      <c r="H28" s="227"/>
+      <c r="I28" s="228"/>
+      <c r="J28" s="228"/>
       <c r="K28" s="145" t="s">
         <v>134</v>
       </c>
@@ -3865,18 +3866,18 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="173" t="s">
+      <c r="A29" s="227" t="s">
         <v>133</v>
       </c>
-      <c r="B29" s="173"/>
-      <c r="C29" s="173"/>
-      <c r="D29" s="173"/>
-      <c r="E29" s="173"/>
-      <c r="F29" s="173"/>
-      <c r="G29" s="173"/>
-      <c r="H29" s="173"/>
-      <c r="I29" s="174"/>
-      <c r="J29" s="174"/>
+      <c r="B29" s="227"/>
+      <c r="C29" s="227"/>
+      <c r="D29" s="227"/>
+      <c r="E29" s="227"/>
+      <c r="F29" s="227"/>
+      <c r="G29" s="227"/>
+      <c r="H29" s="227"/>
+      <c r="I29" s="228"/>
+      <c r="J29" s="228"/>
       <c r="K29" s="145" t="s">
         <v>129</v>
       </c>
@@ -3886,18 +3887,18 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="173" t="s">
+      <c r="A30" s="227" t="s">
         <v>132</v>
       </c>
-      <c r="B30" s="173"/>
-      <c r="C30" s="173"/>
-      <c r="D30" s="173"/>
-      <c r="E30" s="173"/>
-      <c r="F30" s="173"/>
-      <c r="G30" s="173"/>
-      <c r="H30" s="173"/>
-      <c r="I30" s="174"/>
-      <c r="J30" s="174"/>
+      <c r="B30" s="227"/>
+      <c r="C30" s="227"/>
+      <c r="D30" s="227"/>
+      <c r="E30" s="227"/>
+      <c r="F30" s="227"/>
+      <c r="G30" s="227"/>
+      <c r="H30" s="227"/>
+      <c r="I30" s="228"/>
+      <c r="J30" s="228"/>
       <c r="K30" s="145" t="s">
         <v>131</v>
       </c>
@@ -3907,21 +3908,21 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="173" t="s">
+      <c r="A31" s="227" t="s">
         <v>130</v>
       </c>
-      <c r="B31" s="173"/>
-      <c r="C31" s="173"/>
-      <c r="D31" s="173"/>
-      <c r="E31" s="173"/>
-      <c r="F31" s="173"/>
-      <c r="G31" s="173"/>
-      <c r="H31" s="173"/>
-      <c r="I31" s="175">
+      <c r="B31" s="227"/>
+      <c r="C31" s="227"/>
+      <c r="D31" s="227"/>
+      <c r="E31" s="227"/>
+      <c r="F31" s="227"/>
+      <c r="G31" s="227"/>
+      <c r="H31" s="227"/>
+      <c r="I31" s="232">
         <f>L19</f>
         <v>0</v>
       </c>
-      <c r="J31" s="175"/>
+      <c r="J31" s="232"/>
       <c r="K31" s="145" t="s">
         <v>129</v>
       </c>
@@ -3943,14 +3944,14 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="13.9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F33" s="170" t="s">
+      <c r="F33" s="229" t="s">
         <v>127</v>
       </c>
-      <c r="G33" s="171"/>
-      <c r="H33" s="171"/>
-      <c r="I33" s="171"/>
-      <c r="J33" s="171"/>
-      <c r="K33" s="172"/>
+      <c r="G33" s="230"/>
+      <c r="H33" s="230"/>
+      <c r="I33" s="230"/>
+      <c r="J33" s="230"/>
+      <c r="K33" s="231"/>
       <c r="L33" s="140">
         <f>L32/10</f>
         <v>0</v>
@@ -4044,23 +4045,26 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I11:L11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="F33:K33"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="B18:J18"/>
+    <mergeCell ref="A21:L25"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
     <mergeCell ref="K13:K15"/>
     <mergeCell ref="L13:L15"/>
     <mergeCell ref="C14:E14"/>
@@ -4070,26 +4074,23 @@
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="J13:J15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="B18:J18"/>
-    <mergeCell ref="A21:L25"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="F33:K33"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="A30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="I8:L8"/>
   </mergeCells>
   <conditionalFormatting sqref="L13:L37 I31:J31">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
@@ -4121,8 +4122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" view="pageLayout" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView showZeros="0" view="pageLayout" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -4191,10 +4192,10 @@
         <v>13</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="235"/>
-      <c r="D5" s="235"/>
-      <c r="E5" s="235"/>
-      <c r="F5" s="235"/>
+      <c r="C5" s="263"/>
+      <c r="D5" s="263"/>
+      <c r="E5" s="263"/>
+      <c r="F5" s="263"/>
       <c r="H5" s="30"/>
       <c r="I5" s="31" t="s">
         <v>11</v>
@@ -4226,10 +4227,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="235"/>
-      <c r="D8" s="235"/>
-      <c r="E8" s="235"/>
-      <c r="F8" s="235"/>
+      <c r="C8" s="263"/>
+      <c r="D8" s="263"/>
+      <c r="E8" s="263"/>
+      <c r="F8" s="263"/>
       <c r="H8" s="4" t="s">
         <v>15</v>
       </c>
@@ -4243,30 +4244,30 @@
         <v>17</v>
       </c>
       <c r="B9" s="4"/>
-      <c r="C9" s="235"/>
-      <c r="D9" s="235"/>
-      <c r="E9" s="235"/>
-      <c r="F9" s="235"/>
+      <c r="C9" s="263"/>
+      <c r="D9" s="263"/>
+      <c r="E9" s="263"/>
+      <c r="F9" s="263"/>
       <c r="H9" s="27"/>
-      <c r="I9" s="242"/>
-      <c r="J9" s="243"/>
-      <c r="K9" s="243"/>
-      <c r="L9" s="243"/>
+      <c r="I9" s="233"/>
+      <c r="J9" s="234"/>
+      <c r="K9" s="234"/>
+      <c r="L9" s="234"/>
     </row>
     <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="4"/>
-      <c r="C10" s="235"/>
-      <c r="D10" s="235"/>
-      <c r="E10" s="235"/>
-      <c r="F10" s="235"/>
+      <c r="C10" s="263"/>
+      <c r="D10" s="263"/>
+      <c r="E10" s="263"/>
+      <c r="F10" s="263"/>
       <c r="H10" s="27"/>
-      <c r="I10" s="242"/>
-      <c r="J10" s="243"/>
-      <c r="K10" s="243"/>
-      <c r="L10" s="243"/>
+      <c r="I10" s="233"/>
+      <c r="J10" s="234"/>
+      <c r="K10" s="234"/>
+      <c r="L10" s="234"/>
     </row>
     <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="94"/>
@@ -4287,215 +4288,215 @@
       <c r="E12" s="35"/>
       <c r="F12" s="35"/>
       <c r="G12" s="35"/>
-      <c r="H12" s="219" t="s">
+      <c r="H12" s="187" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="220"/>
-      <c r="J12" s="221" t="s">
+      <c r="I12" s="188"/>
+      <c r="J12" s="189" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="222"/>
-      <c r="L12" s="223"/>
+      <c r="K12" s="190"/>
+      <c r="L12" s="191"/>
     </row>
     <row r="13" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="246" t="s">
+      <c r="A13" s="248" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="241" t="s">
+      <c r="B13" s="252" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="241" t="s">
+      <c r="C13" s="252" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="241"/>
-      <c r="E13" s="241"/>
-      <c r="F13" s="262" t="s">
+      <c r="D13" s="252"/>
+      <c r="E13" s="252"/>
+      <c r="F13" s="240" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="263"/>
+      <c r="G13" s="241"/>
       <c r="H13" s="36"/>
       <c r="I13" s="37"/>
-      <c r="J13" s="239" t="s">
+      <c r="J13" s="242" t="s">
         <v>6</v>
       </c>
       <c r="K13" s="244"/>
-      <c r="L13" s="261">
+      <c r="L13" s="239">
         <f>ROUND(K13*0.3,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="247"/>
-      <c r="B14" s="250"/>
-      <c r="C14" s="250" t="s">
+      <c r="A14" s="249"/>
+      <c r="B14" s="254"/>
+      <c r="C14" s="254" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="250"/>
-      <c r="E14" s="250"/>
-      <c r="F14" s="208" t="s">
+      <c r="D14" s="254"/>
+      <c r="E14" s="254"/>
+      <c r="F14" s="197" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="209"/>
+      <c r="G14" s="198"/>
       <c r="H14" s="38"/>
       <c r="I14" s="39"/>
-      <c r="J14" s="240"/>
+      <c r="J14" s="243"/>
       <c r="K14" s="245"/>
-      <c r="L14" s="259"/>
+      <c r="L14" s="237"/>
     </row>
     <row r="15" spans="1:13" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="247"/>
-      <c r="B15" s="250"/>
-      <c r="C15" s="250" t="s">
+      <c r="A15" s="249"/>
+      <c r="B15" s="254"/>
+      <c r="C15" s="254" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="250"/>
-      <c r="E15" s="250"/>
-      <c r="F15" s="208" t="s">
+      <c r="D15" s="254"/>
+      <c r="E15" s="254"/>
+      <c r="F15" s="197" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="209"/>
+      <c r="G15" s="198"/>
       <c r="H15" s="40"/>
       <c r="I15" s="41"/>
-      <c r="J15" s="240"/>
+      <c r="J15" s="243"/>
       <c r="K15" s="245"/>
-      <c r="L15" s="259"/>
+      <c r="L15" s="237"/>
     </row>
     <row r="16" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="247"/>
-      <c r="B16" s="251" t="s">
+      <c r="A16" s="249"/>
+      <c r="B16" s="255" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="250" t="s">
+      <c r="C16" s="254" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="250"/>
-      <c r="E16" s="250"/>
-      <c r="F16" s="208" t="s">
+      <c r="D16" s="254"/>
+      <c r="E16" s="254"/>
+      <c r="F16" s="197" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="209"/>
+      <c r="G16" s="198"/>
       <c r="H16" s="42"/>
       <c r="I16" s="43"/>
-      <c r="J16" s="240" t="s">
+      <c r="J16" s="243" t="s">
         <v>7</v>
       </c>
       <c r="K16" s="245"/>
-      <c r="L16" s="259">
+      <c r="L16" s="237">
         <f>ROUND(K16*0.25,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="247"/>
-      <c r="B17" s="252"/>
-      <c r="C17" s="250" t="s">
+      <c r="A17" s="249"/>
+      <c r="B17" s="256"/>
+      <c r="C17" s="254" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="250"/>
-      <c r="E17" s="250"/>
-      <c r="F17" s="208" t="s">
+      <c r="D17" s="254"/>
+      <c r="E17" s="254"/>
+      <c r="F17" s="197" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="209"/>
+      <c r="G17" s="198"/>
       <c r="H17" s="38"/>
       <c r="I17" s="39"/>
-      <c r="J17" s="240"/>
+      <c r="J17" s="243"/>
       <c r="K17" s="245"/>
-      <c r="L17" s="259"/>
+      <c r="L17" s="237"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="248"/>
-      <c r="B18" s="253"/>
-      <c r="C18" s="236" t="s">
+      <c r="A18" s="250"/>
+      <c r="B18" s="257"/>
+      <c r="C18" s="251" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="236"/>
-      <c r="E18" s="236"/>
-      <c r="F18" s="200" t="s">
+      <c r="D18" s="251"/>
+      <c r="E18" s="251"/>
+      <c r="F18" s="213" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="201"/>
+      <c r="G18" s="214"/>
       <c r="H18" s="44"/>
       <c r="I18" s="45"/>
-      <c r="J18" s="264"/>
-      <c r="K18" s="265"/>
-      <c r="L18" s="260"/>
+      <c r="J18" s="246"/>
+      <c r="K18" s="247"/>
+      <c r="L18" s="238"/>
     </row>
     <row r="19" spans="1:12" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="246" t="s">
+      <c r="A19" s="248" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="254" t="s">
+      <c r="B19" s="258" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="241" t="s">
+      <c r="C19" s="252" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="241"/>
-      <c r="E19" s="241"/>
-      <c r="F19" s="237" t="s">
+      <c r="D19" s="252"/>
+      <c r="E19" s="252"/>
+      <c r="F19" s="264" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="238"/>
+      <c r="G19" s="265"/>
       <c r="H19" s="46"/>
       <c r="I19" s="47"/>
-      <c r="J19" s="239" t="s">
+      <c r="J19" s="242" t="s">
         <v>77</v>
       </c>
       <c r="K19" s="244"/>
-      <c r="L19" s="261">
+      <c r="L19" s="239">
         <f>ROUND(K19*0.25,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="247"/>
-      <c r="B20" s="255"/>
-      <c r="C20" s="250" t="s">
+      <c r="A20" s="249"/>
+      <c r="B20" s="259"/>
+      <c r="C20" s="254" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="250"/>
-      <c r="E20" s="250"/>
-      <c r="F20" s="208" t="s">
+      <c r="D20" s="254"/>
+      <c r="E20" s="254"/>
+      <c r="F20" s="197" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="209"/>
+      <c r="G20" s="198"/>
       <c r="H20" s="38"/>
       <c r="I20" s="39"/>
-      <c r="J20" s="240"/>
+      <c r="J20" s="243"/>
       <c r="K20" s="245"/>
-      <c r="L20" s="259"/>
+      <c r="L20" s="237"/>
     </row>
     <row r="21" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="247"/>
-      <c r="B21" s="256"/>
-      <c r="C21" s="250" t="s">
+      <c r="A21" s="249"/>
+      <c r="B21" s="260"/>
+      <c r="C21" s="254" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="250"/>
-      <c r="E21" s="250"/>
-      <c r="F21" s="208" t="s">
+      <c r="D21" s="254"/>
+      <c r="E21" s="254"/>
+      <c r="F21" s="197" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="209"/>
+      <c r="G21" s="198"/>
       <c r="H21" s="40"/>
       <c r="I21" s="41"/>
-      <c r="J21" s="240"/>
+      <c r="J21" s="243"/>
       <c r="K21" s="245"/>
-      <c r="L21" s="259"/>
+      <c r="L21" s="237"/>
     </row>
     <row r="22" spans="1:12" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="248"/>
+      <c r="A22" s="250"/>
       <c r="B22" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="236"/>
-      <c r="D22" s="236"/>
-      <c r="E22" s="236"/>
-      <c r="F22" s="200" t="s">
+      <c r="C22" s="251"/>
+      <c r="D22" s="251"/>
+      <c r="E22" s="251"/>
+      <c r="F22" s="213" t="s">
         <v>44</v>
       </c>
-      <c r="G22" s="201"/>
+      <c r="G22" s="214"/>
       <c r="H22" s="49"/>
       <c r="I22" s="50"/>
       <c r="J22" s="51" t="s">
@@ -4514,15 +4515,15 @@
       <c r="B23" s="97" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="249" t="s">
+      <c r="C23" s="253" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="249"/>
-      <c r="E23" s="249"/>
-      <c r="F23" s="257" t="s">
+      <c r="D23" s="253"/>
+      <c r="E23" s="253"/>
+      <c r="F23" s="235" t="s">
         <v>47</v>
       </c>
-      <c r="G23" s="258"/>
+      <c r="G23" s="236"/>
       <c r="H23" s="53"/>
       <c r="I23" s="54"/>
       <c r="J23" s="55" t="s">
@@ -4561,11 +4562,11 @@
         <v>9</v>
       </c>
       <c r="J25" s="25"/>
-      <c r="K25" s="233">
+      <c r="K25" s="261">
         <f>SUM(L13:L23)</f>
         <v>0</v>
       </c>
-      <c r="L25" s="234"/>
+      <c r="L25" s="262"/>
     </row>
     <row r="28" spans="1:12" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A28"/>
@@ -4615,35 +4616,6 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="L16:L18"/>
-    <mergeCell ref="L13:L15"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="J19:J21"/>
-    <mergeCell ref="K19:K21"/>
-    <mergeCell ref="L19:L21"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="J16:J18"/>
-    <mergeCell ref="K16:K18"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A13:A18"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="B13:B15"/>
     <mergeCell ref="K25:L25"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C8:F8"/>
@@ -4660,12 +4632,41 @@
     <mergeCell ref="J12:L12"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="C9:F9"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A13:A18"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="L16:L18"/>
+    <mergeCell ref="L13:L15"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="J19:J21"/>
+    <mergeCell ref="K19:K21"/>
+    <mergeCell ref="L19:L21"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="J16:J18"/>
+    <mergeCell ref="K16:K18"/>
+    <mergeCell ref="F17:G17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;G&amp;C&amp;"Verdana,Normal"&amp;12PROTOKOLL FÖR SKRITT PAS-DE-DEUX</oddHeader>
-    <oddFooter>&amp;R2019-04-07</oddFooter>
+    <oddFooter>&amp;R2019-06-01</oddFooter>
   </headerFooter>
   <legacyDrawingHF r:id="rId2"/>
 </worksheet>
@@ -4675,8 +4676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" view="pageLayout" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView showZeros="0" view="pageLayout" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -4742,10 +4743,10 @@
         <v>13</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="235"/>
-      <c r="D5" s="235"/>
-      <c r="E5" s="235"/>
-      <c r="F5" s="235"/>
+      <c r="C5" s="263"/>
+      <c r="D5" s="263"/>
+      <c r="E5" s="263"/>
+      <c r="F5" s="263"/>
       <c r="H5" s="30"/>
       <c r="I5" s="31" t="s">
         <v>11</v>
@@ -4799,30 +4800,30 @@
         <v>17</v>
       </c>
       <c r="B9" s="4"/>
-      <c r="C9" s="235"/>
-      <c r="D9" s="235"/>
-      <c r="E9" s="235"/>
-      <c r="F9" s="235"/>
+      <c r="C9" s="263"/>
+      <c r="D9" s="263"/>
+      <c r="E9" s="263"/>
+      <c r="F9" s="263"/>
       <c r="H9" s="27"/>
-      <c r="I9" s="242"/>
-      <c r="J9" s="243"/>
-      <c r="K9" s="243"/>
-      <c r="L9" s="243"/>
+      <c r="I9" s="233"/>
+      <c r="J9" s="234"/>
+      <c r="K9" s="234"/>
+      <c r="L9" s="234"/>
     </row>
     <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="4"/>
-      <c r="C10" s="235"/>
-      <c r="D10" s="235"/>
-      <c r="E10" s="235"/>
-      <c r="F10" s="235"/>
+      <c r="C10" s="263"/>
+      <c r="D10" s="263"/>
+      <c r="E10" s="263"/>
+      <c r="F10" s="263"/>
       <c r="H10" s="27"/>
-      <c r="I10" s="242"/>
-      <c r="J10" s="243"/>
-      <c r="K10" s="243"/>
-      <c r="L10" s="243"/>
+      <c r="I10" s="233"/>
+      <c r="J10" s="234"/>
+      <c r="K10" s="234"/>
+      <c r="L10" s="234"/>
     </row>
     <row r="11" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -4887,12 +4888,17 @@
       </c>
       <c r="C18" s="28"/>
       <c r="D18" s="15"/>
-      <c r="E18" s="123"/>
+      <c r="E18" s="123">
+        <v>0</v>
+      </c>
       <c r="F18" s="89">
         <v>0.8</v>
       </c>
       <c r="G18" s="90"/>
-      <c r="H18" s="123"/>
+      <c r="H18" s="279">
+        <f>IF(E18&gt;12,13,E18)</f>
+        <v>0</v>
+      </c>
       <c r="I18" s="91"/>
       <c r="J18" s="92"/>
       <c r="K18" s="64">
@@ -4906,12 +4912,17 @@
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="15"/>
-      <c r="E19" s="123"/>
+      <c r="E19" s="123">
+        <v>0</v>
+      </c>
       <c r="F19" s="89">
         <v>0.4</v>
       </c>
       <c r="G19" s="90"/>
-      <c r="H19" s="123"/>
+      <c r="H19" s="279">
+        <f>IF(SUM(E18:E19)&gt;12,13-H18,E19)</f>
+        <v>0</v>
+      </c>
       <c r="I19" s="91"/>
       <c r="J19" s="92"/>
       <c r="K19" s="64">
@@ -4925,12 +4936,17 @@
       </c>
       <c r="C20" s="28"/>
       <c r="D20" s="15"/>
-      <c r="E20" s="123"/>
+      <c r="E20" s="123">
+        <v>0</v>
+      </c>
       <c r="F20" s="89">
         <v>0</v>
       </c>
       <c r="G20" s="90"/>
-      <c r="H20" s="123"/>
+      <c r="H20" s="279">
+        <f>IF(SUM(E18:E20)&gt;12,IF(13-SUM(H18:H19)&gt;0,13-SUM(H18:H19),0),E20)</f>
+        <v>0</v>
+      </c>
       <c r="I20" s="91"/>
       <c r="J20" s="92"/>
       <c r="K20" s="64">
@@ -5095,7 +5111,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;G&amp;C&amp;"Verdana,Normal"&amp;12PROTOKOLL FÖR SKRITT PAS-DE-DEUX</oddHeader>
-    <oddFooter>&amp;R2019-04-07</oddFooter>
+    <oddFooter>&amp;R2019-06-01</oddFooter>
   </headerFooter>
   <legacyDrawingHF r:id="rId2"/>
 </worksheet>
@@ -5105,8 +5121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" view="pageLayout" topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView showZeros="0" tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -5173,10 +5189,10 @@
         <v>13</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="235"/>
-      <c r="D5" s="235"/>
-      <c r="E5" s="235"/>
-      <c r="F5" s="235"/>
+      <c r="C5" s="263"/>
+      <c r="D5" s="263"/>
+      <c r="E5" s="263"/>
+      <c r="F5" s="263"/>
       <c r="H5" s="30"/>
       <c r="I5" s="31" t="s">
         <v>11</v>
@@ -5236,30 +5252,30 @@
         <v>17</v>
       </c>
       <c r="B9" s="4"/>
-      <c r="C9" s="235"/>
-      <c r="D9" s="235"/>
-      <c r="E9" s="235"/>
-      <c r="F9" s="235"/>
+      <c r="C9" s="263"/>
+      <c r="D9" s="263"/>
+      <c r="E9" s="263"/>
+      <c r="F9" s="263"/>
       <c r="H9" s="27"/>
-      <c r="I9" s="242"/>
-      <c r="J9" s="243"/>
-      <c r="K9" s="243"/>
-      <c r="L9" s="243"/>
+      <c r="I9" s="233"/>
+      <c r="J9" s="234"/>
+      <c r="K9" s="234"/>
+      <c r="L9" s="234"/>
     </row>
     <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="4"/>
-      <c r="C10" s="235"/>
-      <c r="D10" s="235"/>
-      <c r="E10" s="235"/>
-      <c r="F10" s="235"/>
+      <c r="C10" s="263"/>
+      <c r="D10" s="263"/>
+      <c r="E10" s="263"/>
+      <c r="F10" s="263"/>
       <c r="H10" s="27"/>
-      <c r="I10" s="242"/>
-      <c r="J10" s="243"/>
-      <c r="K10" s="243"/>
-      <c r="L10" s="243"/>
+      <c r="I10" s="233"/>
+      <c r="J10" s="234"/>
+      <c r="K10" s="234"/>
+      <c r="L10" s="234"/>
     </row>
     <row r="11" spans="1:13" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K11" s="14" t="s">
@@ -5436,6 +5452,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="I9:L9"/>
     <mergeCell ref="B15:I15"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A16"/>
@@ -5443,24 +5465,36 @@
     <mergeCell ref="B13:I13"/>
     <mergeCell ref="B14:I14"/>
     <mergeCell ref="B16:I16"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="I9:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;G&amp;C&amp;"Verdana,Normal"&amp;12PROTOKOLL FÖR SKRITT PAS-DE-DEUX</oddHeader>
-    <oddFooter>&amp;R2019-04-07</oddFooter>
+    <oddFooter>&amp;R2019-06-01</oddFooter>
   </headerFooter>
   <legacyDrawingHF r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100570C130F412EDB4EBF3E80DF6A9149FD" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfaa3b10b9be17ef9f56bd19dc71004c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddb0c952b897a810c8a4e377cff6bff8" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5526,25 +5560,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06F9B768-A93D-4D4C-BBD7-D4CF83092D49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A00BD0D-8423-4FFE-92A4-D273D2078383}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5559,27 +5598,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06F9B768-A93D-4D4C-BBD7-D4CF83092D49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>